<commit_message>
code in tangsengjiewa-second times
</commit_message>
<xml_diff>
--- a/Revit二次开发笔记.xlsx
+++ b/Revit二次开发笔记.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\githubRep2\Gitee500LinesEveryday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA92AE4-C739-4EB0-ACB8-8171874998E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE79C318-5DD3-4444-AB6E-6569AC8F0745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8088" yWindow="1776" windowWidth="16512" windowHeight="9420" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01任务列表" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="1451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="1455">
   <si>
     <t>attribute  和 property</t>
   </si>
@@ -12218,6 +12218,21 @@
       </rPr>
       <t>.</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Autodesk.Revit.DB.Transform 类的作用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revit 提供了Transform类来做二次开发时的坐标转换。 你可以给Transform对象进行赋值，构造一个变换矩阵。然后使用这个变化矩阵把给定的坐标点的坐标转成目标坐标系。</t>
+  </si>
+  <si>
+    <t>当然你可以使用第三方的代码做纯粹的坐标转换功能。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -12940,7 +12955,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="CAEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -13601,10 +13616,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M202"/>
+  <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14775,34 +14790,52 @@
         <v>837</v>
       </c>
     </row>
-    <row r="193" spans="2:4">
+    <row r="193" spans="2:8">
       <c r="B193" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="2:8">
       <c r="D194" t="s">
         <v>1014</v>
       </c>
     </row>
-    <row r="195" spans="2:4">
+    <row r="195" spans="2:8">
       <c r="D195" s="27" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="197" spans="2:4">
+    <row r="197" spans="2:8">
       <c r="B197" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="198" spans="2:4">
+    <row r="198" spans="2:8">
       <c r="B198" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="202" spans="2:4" ht="20.399999999999999">
+    <row r="202" spans="2:8" ht="20.399999999999999">
       <c r="B202" s="38" t="s">
         <v>1202</v>
+      </c>
+    </row>
+    <row r="205" spans="2:8" ht="20.399999999999999">
+      <c r="B205" s="38" t="s">
+        <v>1451</v>
+      </c>
+      <c r="H205" s="8" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="206" spans="2:8" ht="15">
+      <c r="C206" s="61" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="207" spans="2:8">
+      <c r="C207" t="s">
+        <v>1454</v>
       </c>
     </row>
   </sheetData>
@@ -14812,9 +14845,10 @@
     <hyperlink ref="D98" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="E163" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="B188" r:id="rId4" display="https://www.cnblogs.com/lonelyxmas/p/10560039.html" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H205" r:id="rId5" xr:uid="{911477FD-CDF5-4536-9EDC-5FD4B17A805C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -14823,7 +14857,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15151,7 +15185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFA973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A943" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A943" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H939" sqref="H939"/>
     </sheetView>
   </sheetViews>
@@ -32696,7 +32730,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="952" spans="2:2">
+    <row r="952" spans="2:2" ht="15">
       <c r="B952" s="26" t="s">
         <v>1433</v>
       </c>
@@ -32726,7 +32760,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="959" spans="2:2">
+    <row r="959" spans="2:2" ht="15">
       <c r="B959" s="26" t="s">
         <v>1439</v>
       </c>
@@ -32881,7 +32915,7 @@
       <c r="L971" s="26"/>
       <c r="M971" s="26"/>
     </row>
-    <row r="972" spans="2:13">
+    <row r="972" spans="2:13" ht="15">
       <c r="C972" s="26" t="s">
         <v>1449</v>
       </c>

</xml_diff>